<commit_message>
Initial algorithm markup established
</commit_message>
<xml_diff>
--- a/data/F03/DB-G4.xlsx
+++ b/data/F03/DB-G4.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="3" documentId="11_FA0F03A837A578D3408040D07942827E5EA1D943" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6BA87A00-187F-43C0-AFCB-2C7AC6404793}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-1608" windowWidth="23256" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Sheet" sheetId="1" r:id="rId1"/>
@@ -574,6 +574,24 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -600,24 +618,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -690,7 +690,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="Header!$A$1:$F$9" spid="_x0000_s1034"/>
+                  <a14:cameraTool cellRange="Header!$A$1:$F$9" spid="_x0000_s1040"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -755,7 +755,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="Summary!$A$37:$F$44" spid="_x0000_s1035"/>
+                  <a14:cameraTool cellRange="Summary!$A$37:$F$44" spid="_x0000_s1041"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -820,7 +820,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="Footer!$A$45:$A$49" spid="_x0000_s1036"/>
+                  <a14:cameraTool cellRange="Footer!$A$45:$A$49" spid="_x0000_s1042"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -1159,17 +1159,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" customWidth="1"/>
-    <col min="2" max="2" width="41.28515625" customWidth="1"/>
-    <col min="3" max="12" width="6.85546875" customWidth="1"/>
-    <col min="13" max="13" width="41.28515625" customWidth="1"/>
-    <col min="14" max="14" width="6.85546875" customWidth="1"/>
+    <col min="1" max="1" width="6.88671875" customWidth="1"/>
+    <col min="2" max="2" width="41.33203125" customWidth="1"/>
+    <col min="3" max="12" width="6.88671875" customWidth="1"/>
+    <col min="13" max="13" width="41.33203125" customWidth="1"/>
+    <col min="14" max="14" width="6.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="27" customHeight="1"/>
@@ -1194,22 +1194,22 @@
       <c r="D10" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="35" t="s">
+      <c r="E10" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="G10" s="35" t="s">
+      <c r="F10" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="I10" s="35" t="s">
+      <c r="H10" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="J10" s="36" t="s">
+      <c r="J10" s="27" t="s">
         <v>5</v>
       </c>
       <c r="K10" s="10" t="s">
@@ -2156,28 +2156,28 @@
       <c r="B32" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C32" s="37" t="s">
+      <c r="C32" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="D32" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="E32" s="39" t="s">
+      <c r="D32" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="F32" s="40" t="s">
-        <v>5</v>
-      </c>
-      <c r="G32" s="39" t="s">
+      <c r="F32" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="G32" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="H32" s="40" t="s">
-        <v>5</v>
-      </c>
-      <c r="I32" s="39" t="s">
+      <c r="H32" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="I32" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="J32" s="40" t="s">
+      <c r="J32" s="31" t="s">
         <v>5</v>
       </c>
       <c r="K32" s="14" t="s">
@@ -2200,28 +2200,28 @@
       <c r="B33" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C33" s="30" t="s">
+      <c r="C33" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="D33" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="E33" s="32" t="s">
+      <c r="D33" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="F33" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="G33" s="32" t="s">
+      <c r="F33" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="G33" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="H33" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="I33" s="32" t="s">
+      <c r="H33" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="I33" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="J33" s="32" t="s">
+      <c r="J33" s="38" t="s">
         <v>5</v>
       </c>
       <c r="K33" s="18" t="s">
@@ -2238,10 +2238,10 @@
       </c>
     </row>
     <row r="34" spans="1:14" ht="13.5" customHeight="1">
-      <c r="A34" s="33" t="s">
+      <c r="A34" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="B34" s="34" t="s">
+      <c r="B34" s="40" t="s">
         <v>5</v>
       </c>
       <c r="C34" s="20" t="s">
@@ -2282,90 +2282,90 @@
       </c>
     </row>
     <row r="35" spans="1:14" ht="13.5" customHeight="1">
-      <c r="A35" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="B35" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="E35" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="F35" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="G35" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="H35" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="I35" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="J35" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="K35" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="L35" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="M35" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="N35" s="28" t="s">
+      <c r="A35" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="F35" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="G35" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="H35" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="I35" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="J35" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="K35" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="L35" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="M35" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="N35" s="34" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="13.5" customHeight="1">
-      <c r="A36" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="B36" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="D36" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="E36" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="F36" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="G36" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="H36" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="I36" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="J36" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="K36" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="L36" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="M36" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="N36" s="28" t="s">
+      <c r="A36" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="E36" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="F36" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="G36" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="H36" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="I36" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="J36" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="K36" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="L36" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="M36" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="N36" s="34" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2384,6 +2384,12 @@
     <row r="49" ht="13.5" customHeight="1"/>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A35:N36"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="A34:B34"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="I10:J10"/>
@@ -2391,12 +2397,6 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="G32:H32"/>
     <mergeCell ref="I32:J32"/>
-    <mergeCell ref="A35:N36"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="A34:B34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2410,14 +2410,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="27.5703125" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" customWidth="1"/>
-    <col min="6" max="6" width="34.42578125" customWidth="1"/>
+    <col min="1" max="1" width="34.44140625" customWidth="1"/>
+    <col min="2" max="2" width="27.5546875" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="4" max="4" width="27.5546875" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" customWidth="1"/>
+    <col min="6" max="6" width="34.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="27" customHeight="1">
@@ -2581,7 +2581,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.5" customHeight="1">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="32" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="42" t="s">
@@ -2615,11 +2615,11 @@
   <sheetViews>
     <sheetView topLeftCell="A37" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="48.140625" customWidth="1"/>
-    <col min="2" max="4" width="20.7109375" customWidth="1"/>
-    <col min="5" max="6" width="27.5703125" customWidth="1"/>
+    <col min="1" max="1" width="48.109375" customWidth="1"/>
+    <col min="2" max="4" width="20.6640625" customWidth="1"/>
+    <col min="5" max="6" width="27.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" hidden="1"/>
@@ -2832,9 +2832,9 @@
   <sheetViews>
     <sheetView topLeftCell="A45" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="165.28515625" customWidth="1"/>
+    <col min="1" max="1" width="165.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" hidden="1"/>

</xml_diff>